<commit_message>
ADN node 9. Flex growth modified
</commit_message>
<xml_diff>
--- a/data/IEEE9/ieee18_3/ieee18_3_2020.xlsx
+++ b/data/IEEE9/ieee18_3/ieee18_3_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\ieee18_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90FCF0F-B7F3-4BB2-92D3-839214CC8F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA8D96E-CCDB-49F1-A4AE-CC318F9AD4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="4965" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14205" yWindow="5385" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -254,7 +254,7 @@
         </row>
         <row r="3">
           <cell r="B3">
-            <v>0.05</v>
+            <v>0.06</v>
           </cell>
         </row>
       </sheetData>
@@ -13486,11 +13486,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5612021857923495E-5</v>
+        <v>3.5248633879781413E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9862241321508028E-5</v>
+        <v>2.1953003565877297E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13510,55 +13510,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3236064726792094E-2</v>
+        <v>3.3914351762032752E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69287252408135513</v>
+        <v>0.67901507359972801</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7110379643844762</v>
+        <v>1.6602150545512739</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3829594203636781</v>
+        <v>2.3148748654961442</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4029369382721901</v>
+        <v>2.6052895225477433</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7845956938630803</v>
+        <v>2.6785158579063912</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4012863004128526</v>
+        <v>2.3551077177126052</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8452558888398061</v>
+        <v>1.9000654696964341</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.99091007020948585</v>
+        <v>0.96118276810320125</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21866933863057539</v>
+        <v>0.22085603201688114</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4486609630193811E-3</v>
+        <v>1.4345962934755037E-3</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3778541182959933E-4</v>
+        <v>2.4513959982432922E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.4642955106519151E-5</v>
+        <v>6.1410807351193193E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13583,23 +13583,23 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.8531822020272304</v>
+        <v>3.6696973352640292</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3025862551929315</v>
+        <v>3.5027429979318976</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4379675738264313</v>
+        <v>3.2415122838934924</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4130165473344172</v>
+        <v>3.1832942797253692</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8988276663537311</v>
+        <v>2.8419879081899326</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13607,11 +13607,11 @@
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1823268280587298</v>
+        <v>2.248457944060509</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9396017519587123</v>
+        <v>2.0187691704060065</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13619,43 +13619,43 @@
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6810549239408505</v>
+        <v>1.7872268138739569</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7746634836737949</v>
+        <v>1.8268594684877302</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6470416584154806</v>
+        <v>1.6643789390303803</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.623343738230008</v>
+        <v>1.5421765513185075</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6795154539955948</v>
+        <v>1.5995385276148522</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0348195522948895</v>
+        <v>2.0146728240543461</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2425735042164998</v>
+        <v>2.1528705640478401</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3202319894433669</v>
+        <v>2.3436686762054211</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6720881965846064</v>
+        <v>2.4645473657819181</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5406924654413761</v>
+        <v>2.4913586311609612</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13663,15 +13663,15 @@
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6285460344715954</v>
+        <v>2.787851854742601</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.588262034465822</v>
+        <v>2.7789760791106723</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5310571056062319</v>
+        <v>2.7156133528900201</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13688,11 +13688,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8714480874316939E-5</v>
+        <v>1.7806010928961748E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0453811221846331E-5</v>
+        <v>1.0871963670720186E-5</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13712,7 +13712,7 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6448460604585883E-2</v>
+        <v>1.6957175881016376E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13720,11 +13720,11 @@
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.88093043710883923</v>
+        <v>0.80469607235903584</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1801322843705835</v>
+        <v>1.1687848585593277</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13732,35 +13732,35 @@
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2596980519856791</v>
+        <v>1.3392579289531956</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1198306304809937</v>
+        <v>1.09674133913087</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.90435808413436036</v>
+        <v>0.94089780470544571</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51527323650893264</v>
+        <v>0.47563683370055321</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10386793584952331</v>
+        <v>0.10714797592898194</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1026581196581302E-4</v>
+        <v>6.8213647287805807E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2502119591040791E-4</v>
+        <v>1.2134410191304296E-4</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2967907104324765E-5</v>
+        <v>3.1675048002194387E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13789,11 +13789,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7260928961748631E-5</v>
+        <v>1.8351092896174861E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0244734997409405E-5</v>
+        <v>9.931120660754014E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13813,47 +13813,47 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7635462916257033E-2</v>
+        <v>1.6109317086965558E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33257881155905045</v>
+        <v>0.34643626204067757</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.86398946716443847</v>
+        <v>0.8894009220810396</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1120477295030498</v>
+        <v>1.1007003036917942</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2267625421705393</v>
+        <v>1.2520566152049835</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3525179084477819</v>
+        <v>1.3922978469315401</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1082859848059319</v>
+        <v>1.1544645675061791</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.92262794441990303</v>
+        <v>0.87695329370604636</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.48554593440264804</v>
+        <v>0.50536413580683781</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10605462923582906</v>
+        <v>0.10714797592898194</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1026581196581302E-4</v>
+        <v>7.2433048150969054E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13861,7 +13861,7 @@
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0705403675596596E-5</v>
+        <v>3.1351833226661785E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13890,7 +13890,7 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9077868852459015E-5</v>
+        <v>1.8351092896174861E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13914,31 +13914,31 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6109317086965558E-2</v>
+        <v>1.6957175881016376E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33950753679986401</v>
+        <v>0.35682934990189791</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83857801224783735</v>
+        <v>0.83010752727563697</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1347425811255609</v>
+        <v>1.1460900069368165</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2014684691360951</v>
+        <v>1.2394095786877612</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2862180109748513</v>
+        <v>1.2729580314802651</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1313752761560556</v>
+        <v>1.1082859848059319</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13946,23 +13946,23 @@
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.48059138405160062</v>
+        <v>0.52022778685998006</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11152136270159345</v>
+        <v>0.10496128254267618</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.8213647287805807E-4</v>
+        <v>6.6807180333418054E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1644130991655637E-4</v>
+        <v>1.1766700791567802E-4</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1351833226661785E-5</v>
+        <v>3.3291121879857366E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14160,11 +14160,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5975409836065571E-5</v>
+        <v>3.5248633879781413E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9862241321508028E-5</v>
+        <v>2.0698546219255736E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14184,55 +14184,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.425349527965308E-2</v>
+        <v>3.5610069350134388E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70672997456298225</v>
+        <v>0.66515762311810089</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6940969944400754</v>
+        <v>1.7449199042732777</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3829594203636781</v>
+        <v>2.1787057557610767</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4029369382721901</v>
+        <v>2.5041132304099669</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7580757348739082</v>
+        <v>2.7050358168955637</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2627505523121112</v>
+        <v>2.3781970090627289</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7904463079831781</v>
+        <v>1.8817956094108914</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0404555737199601</v>
+        <v>0.95127366740110642</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21210925847165812</v>
+        <v>0.2230427254031869</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3502082762122387E-3</v>
+        <v>1.420531623931626E-3</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5249378781905908E-4</v>
+        <v>2.4513959982432922E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.528938465758434E-5</v>
+        <v>6.4642955106519151E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14261,11 +14261,11 @@
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4026646265624145</v>
+        <v>3.3025862551929315</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2742548322156493</v>
+        <v>3.3069973805378057</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14273,51 +14273,51 @@
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9556674245175301</v>
+        <v>2.8704077872718319</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3829501568181675</v>
+        <v>2.5334522719856309</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.248457944060509</v>
+        <v>2.3145890600622891</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9989773157941828</v>
+        <v>1.8802261881232414</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8795872227872299</v>
+        <v>1.9958503499699458</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7518361838962548</v>
+        <v>1.8403127588405104</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.75726482206915</v>
+        <v>1.7224674988598596</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6817162196452802</v>
+        <v>1.7684026227197791</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7045109251415083</v>
+        <v>1.6720440503769081</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6635200687194462</v>
+        <v>1.5195616012341095</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9945260958138027</v>
+        <v>1.9743793675732593</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3547021794273251</v>
+        <v>2.1304448290056746</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14325,31 +14325,31 @@
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7239734042852786</v>
+        <v>2.6202029888839347</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4913586311609612</v>
+        <v>2.4173578797403383</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5238971143065578</v>
+        <v>2.5996140277357549</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7613008846974338</v>
+        <v>2.5223421542909246</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6155068979865153</v>
+        <v>2.7244863520692864</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6628829965232237</v>
+        <v>2.7156133528900201</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9496598262223568</v>
+        <v>3.098632544718436</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -14366,7 +14366,7 @@
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0035658772972477E-5</v>
+        <v>1.0662887446283258E-5</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14386,35 +14386,35 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6787604122206212E-2</v>
+        <v>1.7635462916257033E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33257881155905045</v>
+        <v>0.34990062466108435</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83857801224783735</v>
+        <v>0.8894009220810396</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1574374327480721</v>
+        <v>1.1007003036917942</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2141155056533173</v>
+        <v>1.2899977247566496</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2994779904694373</v>
+        <v>1.3657778879423679</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1082859848059319</v>
+        <v>1.1775538588563026</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.9134930142771317</v>
+        <v>0.93176287456267437</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14422,19 +14422,19 @@
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10824132262213482</v>
+        <v>0.11042801600844057</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1729814673775183E-4</v>
+        <v>6.7510413810611936E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2624689390952954E-4</v>
+        <v>1.2011840391392132E-4</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.264469232879217E-5</v>
+        <v>3.361433665538996E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14463,11 +14463,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8714480874316939E-5</v>
+        <v>1.7806010928961748E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0662887446283258E-5</v>
+        <v>1.0349273109627868E-5</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14487,11 +14487,11 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6278888845775719E-2</v>
+        <v>1.7465891157446869E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32911444893864367</v>
+        <v>0.36029371252230469</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14499,7 +14499,7 @@
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1007003036917942</v>
+        <v>1.1460900069368165</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14507,35 +14507,35 @@
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3790378674369541</v>
+        <v>1.2994779904694373</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1429199218311172</v>
+        <v>1.166009213181241</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.88608822384881769</v>
+        <v>0.95003273484821704</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.52022778685998006</v>
+        <v>0.48554593440264804</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10605462923582906</v>
+        <v>0.11261470939474633</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1729814673775183E-4</v>
+        <v>6.8916880764999678E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2134410191304296E-4</v>
+        <v>1.2502119591040791E-4</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.264469232879217E-5</v>
+        <v>3.1028618451129191E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14564,11 +14564,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8714480874316939E-5</v>
+        <v>1.7806010928961748E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0140196885190942E-5</v>
+        <v>1.0871963670720186E-5</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14588,55 +14588,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6109317086965558E-2</v>
+        <v>1.6787604122206212E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33257881155905045</v>
+        <v>0.34990062466108435</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83857801224783735</v>
+        <v>0.80469607235903584</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1120477295030498</v>
+        <v>1.0893528778805384</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2141155056533173</v>
+        <v>1.2647036517222054</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3127379699640236</v>
+        <v>1.3790378674369541</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1890985045313645</v>
+        <v>1.166009213181241</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.9134930142771317</v>
+        <v>0.87695329370604636</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51527323650893264</v>
+        <v>0.49545503510474292</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10605462923582906</v>
+        <v>0.10386793584952331</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.6807180333418054E-4</v>
+        <v>6.8916880764999678E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2502119591040791E-4</v>
+        <v>1.2134410191304296E-4</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.264469232879217E-5</v>
+        <v>3.3937551430922555E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14834,11 +14834,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4521857923497262E-5</v>
+        <v>3.6702185792349721E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0698546219255736E-5</v>
+        <v>2.1743927341440371E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14858,23 +14858,23 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5270925832514066E-2</v>
+        <v>3.5610069350134388E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69287252408135513</v>
+        <v>0.71365869980379582</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7110379643844762</v>
+        <v>1.6093921447180717</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2240954590060995</v>
+        <v>2.3829594203636781</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4029369382721901</v>
+        <v>2.6052895225477433</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14882,27 +14882,27 @@
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2627505523121112</v>
+        <v>2.3320184263624819</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8269860285542634</v>
+        <v>1.8087161682687207</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0206373723157705</v>
+        <v>0.97109186880529608</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.20773587169904661</v>
+        <v>0.21648264524426963</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3502082762122387E-3</v>
+        <v>1.3642729457561161E-3</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4513959982432922E-4</v>
+        <v>2.3778541182959933E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14931,59 +14931,59 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6330003619113884</v>
+        <v>3.7063943086166695</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3359457123160929</v>
+        <v>3.4026646265624145</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3069973805378057</v>
+        <v>3.2742548322156493</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4130165473344172</v>
+        <v>3.2817466801292472</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.699888512780436</v>
+        <v>2.8704077872718319</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.483284900263143</v>
+        <v>2.5585359578468747</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2925453547283627</v>
+        <v>2.1382394173908761</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0781447342414774</v>
+        <v>2.0385610250178301</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8408328470596582</v>
+        <v>2.0346047256975175</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7164455539185526</v>
+        <v>1.8226174438516591</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6876701756505694</v>
+        <v>1.7050688372552147</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6643789390303803</v>
+        <v>1.8204144645644784</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5746434260831075</v>
+        <v>1.655810612994608</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5675477570625551</v>
+        <v>1.6635200687194462</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14991,39 +14991,39 @@
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1752962990900047</v>
+        <v>2.1528705640478401</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3202319894433669</v>
+        <v>2.437415423253638</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6720881965846064</v>
+        <v>2.6461455927342707</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3433571283197159</v>
+        <v>2.5160255483011689</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5491360854496232</v>
+        <v>2.4734191720204266</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6285460344715954</v>
+        <v>2.5223421542909246</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.642751761507208</v>
+        <v>2.6699966250279008</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7156133528900201</v>
+        <v>2.7419785310734186</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1284270884176513</v>
+        <v>2.8304816514254942</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -15036,11 +15036,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9077868852459015E-5</v>
+        <v>1.8896174863387977E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0349273109627868E-5</v>
+        <v>1.0035658772972477E-5</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15060,55 +15060,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6957175881016376E-2</v>
+        <v>1.6787604122206212E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33950753679986401</v>
+        <v>0.34643626204067757</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83857801224783735</v>
+        <v>0.86398946716443847</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1120477295030498</v>
+        <v>1.1460900069368165</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2267625421705393</v>
+        <v>1.2520566152049835</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2862180109748513</v>
+        <v>1.3922978469315401</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1429199218311172</v>
+        <v>1.1198306304809937</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.88608822384881769</v>
+        <v>0.86781836356327502</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.48059138405160062</v>
+        <v>0.47068228334950574</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11261470939474633</v>
+        <v>0.10605462923582906</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1729814673775183E-4</v>
+        <v>6.962011424219356E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1766700791567802E-4</v>
+        <v>1.2747259190865119E-4</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.264469232879217E-5</v>
+        <v>3.3291121879857366E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15137,11 +15137,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7624316939890707E-5</v>
+        <v>1.7442622950819669E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0453811221846331E-5</v>
+        <v>1.0976501782938649E-5</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15161,23 +15161,23 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6957175881016376E-2</v>
+        <v>1.6787604122206212E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.36375807514271147</v>
+        <v>0.34297189942027079</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.84704849722003772</v>
+        <v>0.87245995213663885</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1007003036917942</v>
+        <v>1.1347425811255609</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2014684691360951</v>
+        <v>1.2773506882394274</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15185,31 +15185,31 @@
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1890985045313645</v>
+        <v>1.1313752761560556</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.95003273484821704</v>
+        <v>0.87695329370604636</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.52022778685998006</v>
+        <v>0.49545503510474292</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11480140278105208</v>
+        <v>0.10714797592898194</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.8916880764999678E-4</v>
+        <v>6.6807180333418054E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2256979991216461E-4</v>
+        <v>1.2011840391392132E-4</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.264469232879217E-5</v>
+        <v>3.361433665538996E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15238,11 +15238,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8351092896174861E-5</v>
+        <v>1.7624316939890707E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0767425558501721E-5</v>
+        <v>9.931120660754014E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15262,55 +15262,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6957175881016376E-2</v>
+        <v>1.6109317086965558E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.36375807514271147</v>
+        <v>0.34297189942027079</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8894009220810396</v>
+        <v>0.86398946716443847</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1687848585593277</v>
+        <v>1.1233951553143053</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2520566152049835</v>
+        <v>1.3026447612738716</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3127379699640236</v>
+        <v>1.3525179084477819</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1775538588563026</v>
+        <v>1.2121877958814882</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.94089780470544571</v>
+        <v>0.95003273484821704</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51527323650893264</v>
+        <v>0.47068228334950574</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11152136270159345</v>
+        <v>0.11480140278105208</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.7510413810611936E-4</v>
+        <v>6.962011424219356E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2869828990777284E-4</v>
+        <v>1.2747259190865119E-4</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1028618451129191E-5</v>
+        <v>3.2967907104324765E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26461,11 +26461,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.568877049180328E-5</v>
+        <v>4.6611775956284149E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7133912407424339E-5</v>
+        <v>2.687047636463381E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26485,55 +26485,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.0169413566500729E-2</v>
+        <v>4.101508543105864E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.90931141671563309</v>
+        <v>0.83936438466058427</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0495187420132335</v>
+        <v>2.092666505002986</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9649878168595403</v>
+        <v>2.8487137848258324</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2299108019865419</v>
+        <v>3.3578280614711575</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4697247859217333</v>
+        <v>3.4360381375147262</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8607648658967042</v>
+        <v>2.8017800233008958</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2045147660158473</v>
+        <v>2.2504421569745108</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2295191519476927</v>
+        <v>1.2543579226941108</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26385508833420152</v>
+        <v>0.26663251031666679</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6682975958966031E-3</v>
+        <v>1.7561027325227402E-3</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1279038858919264E-4</v>
+        <v>2.8572198957666634E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.5089256651732648E-5</v>
+        <v>7.7435795922099285E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26558,15 +26558,15 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5860228729327908</v>
+        <v>2.6404654597313755</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.39406855012788</v>
+        <v>2.4658906066317163</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6320302015174506</v>
+        <v>2.5066954300166193</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26574,35 +26574,35 @@
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2380654776995721</v>
+        <v>2.1528058404538744</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9982172187606491</v>
+        <v>1.8079108169739206</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6779509734485998</v>
+        <v>1.6437070760312813</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5516458039480563</v>
+        <v>1.5055573147218761</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4363012817897465</v>
+        <v>1.422080477019551</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2942154621974331</v>
+        <v>1.3726527629366716</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3445442646552059</v>
+        <v>1.3046073062991106</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2471336824429935</v>
+        <v>1.3242759720786426</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26610,7 +26610,7 @@
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2275020635087575</v>
+        <v>1.2518090350633864</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26618,19 +26618,19 @@
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7074295075261576</v>
+        <v>1.5902529726959311</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6345447206563244</v>
+        <v>1.6682466736595474</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8272038794085148</v>
+        <v>1.9985042431030633</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8287633076070997</v>
+        <v>1.7201239031947966</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26638,19 +26638,19 @@
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0122879877608928</v>
+        <v>1.9707975137864415</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.015386819564474</v>
+        <v>1.91461747858625</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0147983123207371</v>
+        <v>2.0345512369513323</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1240868222197959</v>
+        <v>2.2582396741494675</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -26663,11 +26663,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1921379781420765E-5</v>
+        <v>2.3998142076502733E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2776648075340586E-5</v>
+        <v>1.356695620371217E-5</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26687,55 +26687,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0084706783250365E-2</v>
+        <v>2.1141796613947755E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.42842557133717324</v>
+        <v>0.45028401885437597</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0786940747438072</v>
+        <v>1.0247593710066167</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5260966704424104</v>
+        <v>1.4970281624339834</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.614955400993271</v>
+        <v>1.5509967712509631</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6338024477398454</v>
+        <v>1.7011757445538596</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5483521181399686</v>
+        <v>1.5336059074910167</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1711484694459189</v>
+        <v>1.1941121649252506</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62096926866045088</v>
+        <v>0.58992080522742829</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.13887109912326395</v>
+        <v>0.14025981011449659</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.8683187992398386E-4</v>
+        <v>8.5170982527352896E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5489139434945597E-4</v>
+        <v>1.4436479473347352E-4</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.0282257474627412E-5</v>
+        <v>3.7935718204260761E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26764,7 +26764,7 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.261363387978142E-5</v>
+        <v>2.1921379781420765E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26788,7 +26788,7 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0930378647808275E-2</v>
+        <v>2.1987468478505665E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26796,23 +26796,23 @@
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0786940747438072</v>
+        <v>1.0571201932489309</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3807541304002759</v>
+        <v>1.3952883844044894</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5509967712509631</v>
+        <v>1.5829760861221172</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7517057171643704</v>
+        <v>1.6338024477398454</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4746210648952083</v>
+        <v>1.4451286435973041</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26820,7 +26820,7 @@
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64580803940686893</v>
+        <v>0.62096926866045088</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26828,15 +26828,15 @@
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.4292931161091531E-4</v>
+        <v>8.3414879794830156E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5489139434945597E-4</v>
+        <v>1.5639519429459632E-4</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.9108987839444087E-5</v>
+        <v>4.0673347353021849E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26865,7 +26865,7 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.284438524590164E-5</v>
+        <v>2.2152131147540982E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26893,23 +26893,23 @@
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.42405388183373272</v>
+        <v>0.45465570835781655</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.046333252501493</v>
+        <v>1.1218418377335595</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3807541304002759</v>
+        <v>1.5115624164381969</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5190174563798093</v>
+        <v>1.5989657435576941</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6338024477398454</v>
+        <v>1.684332420350356</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26917,27 +26917,27 @@
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1826303171855848</v>
+        <v>1.1022573830079236</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62096926866045088</v>
+        <v>0.63338865403365996</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.13470496614956604</v>
+        <v>0.1333162551583334</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.1317342091182491E-4</v>
+        <v>8.6927085259875636E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4887619456889457E-4</v>
+        <v>1.4286099478833317E-4</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.7935718204260761E-5</v>
+        <v>3.9891167596232968E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27216,11 +27216,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.5227267759562839E-5</v>
+        <v>4.568877049180328E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.687047636463381E-5</v>
+        <v>2.5553296150681172E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27240,31 +27240,31 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.2706429160174468E-2</v>
+        <v>4.1860757295616551E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.89182465870187089</v>
+        <v>0.90931141671563309</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.243683675467119</v>
+        <v>2.092666505002986</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8196452768174058</v>
+        <v>2.9068508008426863</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3258487466000037</v>
+        <v>3.1659521722442343</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4360381375147262</v>
+        <v>3.368664840700712</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0377193936841289</v>
+        <v>3.0082269723862249</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27272,15 +27272,15 @@
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2295191519476927</v>
+        <v>1.2916160788137379</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28607446419392374</v>
+        <v>0.2777421982465279</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6858586232218306E-3</v>
+        <v>1.7561027325227402E-3</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27288,7 +27288,7 @@
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.9000155435677061E-5</v>
+        <v>7.665361616531041E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27313,59 +27313,59 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5860228729327908</v>
+        <v>2.6404654597313755</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5137719776342742</v>
+        <v>2.39406855012788</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6069632472172843</v>
+        <v>2.4064276128159543</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4390799908645242</v>
+        <v>2.3666320703437953</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0249163845853273</v>
+        <v>2.2167505683881479</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9601559384033034</v>
+        <v>1.9030640178672849</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7806826657005548</v>
+        <v>1.7978046144092144</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5209201444639362</v>
+        <v>1.5055573147218761</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3936388674791598</v>
+        <v>1.4363012817897465</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3072883456539728</v>
+        <v>1.2549968118278139</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3445442646552059</v>
+        <v>1.3578565841072376</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3242759720786426</v>
+        <v>1.2471336824429935</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2589376442273736</v>
+        <v>1.2349578795754235</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2518090350633864</v>
+        <v>1.1910416061768141</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27377,35 +27377,35 @@
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.685097650161159</v>
+        <v>1.651395697157936</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9985042431030633</v>
+        <v>1.8272038794085148</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7563370379988976</v>
+        <v>1.7744436054009483</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8894864924560189</v>
+        <v>1.9272762223051392</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0537784617353441</v>
+        <v>2.1575046466714727</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9750790831731844</v>
+        <v>2.0758484241514084</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9950453876901415</v>
+        <v>2.0543041615819275</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1688044395296866</v>
+        <v>2.325316100114303</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -27418,11 +27418,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3767390710382512E-5</v>
+        <v>2.1921379781420765E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3698674225107434E-5</v>
+        <v>1.2513212032550058E-5</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27442,15 +27442,15 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.156463254622671E-2</v>
+        <v>2.050754271552932E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44154063984749486</v>
+        <v>0.42842557133717324</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0247593710066167</v>
+        <v>1.0679071339963691</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27458,39 +27458,39 @@
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5989657435576941</v>
+        <v>1.56698642868654</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7517057171643704</v>
+        <v>1.6001157993328381</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4451286435973041</v>
+        <v>1.4893672755441603</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1826303171855848</v>
+        <v>1.1711484694459189</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63959834672026439</v>
+        <v>0.6085498832872418</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.13887109912326395</v>
+        <v>0.13609367714079867</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.6927085259875636E-4</v>
+        <v>9.1317342091182491E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5639519429459632E-4</v>
+        <v>1.4286099478833317E-4</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.8326808082655205E-5</v>
+        <v>3.9108987839444087E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27519,11 +27519,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.422889344262295E-5</v>
+        <v>2.3305887978142075E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3435238182316905E-5</v>
+        <v>1.3171802139526378E-5</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27547,51 +27547,51 @@
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45902739786125707</v>
+        <v>0.42842557133717324</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0571201932489309</v>
+        <v>1.0247593710066167</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3952883844044894</v>
+        <v>1.4388911464171297</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5829760861221172</v>
+        <v>1.56698642868654</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7011757445538596</v>
+        <v>1.6506457719433489</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4598748542462563</v>
+        <v>1.4156362222993999</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1022573830079236</v>
+        <v>1.1481847739665871</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64580803940686893</v>
+        <v>0.65201773209347347</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.14025981011449659</v>
+        <v>0.13192754416710076</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.8683187992398386E-4</v>
+        <v>8.6927085259875636E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4586859467861387E-4</v>
+        <v>1.5489139434945597E-4</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.7935718204260761E-5</v>
+        <v>3.715353844747188E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27620,11 +27620,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3536639344262295E-5</v>
+        <v>2.2382882513661202E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2776648075340586E-5</v>
+        <v>1.3435238182316905E-5</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27644,27 +27644,27 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1987468478505665E-2</v>
+        <v>2.0296124749389844E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45028401885437597</v>
+        <v>0.43716895034405434</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.046333252501493</v>
+        <v>1.0355463117540549</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4098226384087029</v>
+        <v>1.3807541304002759</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.614955400993271</v>
+        <v>1.5989657435576941</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7180190687573631</v>
+        <v>1.7517057171643704</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27672,27 +27672,27 @@
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2055940126649165</v>
+        <v>1.1481847739665871</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.6085498832872418</v>
+        <v>0.62717896134705542</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.14164852110572923</v>
+        <v>0.13887109912326395</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.0439290724921126E-4</v>
+        <v>9.2195393457443866E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5489139434945597E-4</v>
+        <v>1.5338759440431562E-4</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.715353844747188E-5</v>
+        <v>4.1064437231416293E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27890,11 +27890,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.4304262295081964E-5</v>
+        <v>4.568877049180328E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.687047636463381E-5</v>
+        <v>2.5026424065100117E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27914,11 +27914,11 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.0592249498779688E-2</v>
+        <v>4.0169413566500729E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83062100565370323</v>
+        <v>0.90056803770875193</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27926,43 +27926,43 @@
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7615082608005519</v>
+        <v>2.8196452768174058</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0380349127596187</v>
+        <v>3.0700142276307725</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4360381375147262</v>
+        <v>3.334978192293705</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0082269723862249</v>
+        <v>2.8902572871946082</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3882243298505013</v>
+        <v>2.2963695479331743</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2170997665744836</v>
+        <v>1.2916160788137379</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26663251031666679</v>
+        <v>0.28329704221145846</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7736637598479677E-3</v>
+        <v>1.8439078691488773E-3</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9474478924750844E-4</v>
+        <v>3.0677518880863124E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.5089256651732648E-5</v>
+        <v>7.9000155435677061E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27987,59 +27987,59 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7493506333285458</v>
+        <v>2.7221293399292534</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3461871791253222</v>
+        <v>2.2743651226214858</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4314945671161206</v>
+        <v>2.4816284757164531</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5356772182254952</v>
+        <v>2.3183334566633098</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2167505683881479</v>
+        <v>2.2380654776995721</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9982172187606491</v>
+        <v>1.8650027375099392</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6437070760312813</v>
+        <v>1.7464387682832365</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4594688254956965</v>
+        <v>1.5977342931742362</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4931845008705285</v>
+        <v>1.478963696100333</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3726527629366716</v>
+        <v>1.2942154621974331</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2779826673950472</v>
+        <v>1.3046073062991106</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3371330203512508</v>
+        <v>1.27284777898821</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1510287032935986</v>
+        <v>1.1390388209676237</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1788881203994996</v>
+        <v>1.1910416061768141</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -28047,19 +28047,19 @@
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5902529726959311</v>
+        <v>1.7074295075261576</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7187996031643822</v>
+        <v>1.7019486266627708</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9033373743838697</v>
+        <v>1.8843040006400309</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7925501728029987</v>
+        <v>1.8649764424112008</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -28067,19 +28067,19 @@
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1575046466714727</v>
+        <v>2.1160141726970214</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0960022923470527</v>
+        <v>2.0556945559557631</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0740570862125232</v>
+        <v>1.9357866137983548</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2805984828044124</v>
+        <v>2.2582396741494675</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -28092,11 +28092,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3767390710382512E-5</v>
+        <v>2.422889344262295E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3698674225107434E-5</v>
+        <v>1.2644930053945321E-5</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28116,47 +28116,47 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.156463254622671E-2</v>
+        <v>2.0296124749389844E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45902739786125707</v>
+        <v>0.43716895034405434</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1218418377335595</v>
+        <v>1.0786940747438072</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4098226384087029</v>
+        <v>1.3952883844044894</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5190174563798093</v>
+        <v>1.5829760861221172</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.684332420350356</v>
+        <v>1.6338024477398454</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5188596968420645</v>
+        <v>1.5041134861931125</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0907755352682578</v>
+        <v>1.1137392307475895</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62096926866045088</v>
+        <v>0.61475957597384634</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.13887109912326395</v>
+        <v>0.14164852110572923</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.6927085259875636E-4</v>
+        <v>8.4292931161091531E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28164,7 +28164,7 @@
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.7544628325866324E-5</v>
+        <v>4.0673347353021849E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28193,11 +28193,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1921379781420765E-5</v>
+        <v>2.261363387978142E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2644930053945321E-5</v>
+        <v>1.3830392246502697E-5</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28217,35 +28217,35 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0718960681668799E-2</v>
+        <v>2.1987468478505665E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.42842557133717324</v>
+        <v>0.42405388183373272</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1110548969861214</v>
+        <v>1.1218418377335595</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4534254004213432</v>
+        <v>1.5115624164381969</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5829760861221172</v>
+        <v>1.614955400993271</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6169591235363416</v>
+        <v>1.6338024477398454</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5336059074910167</v>
+        <v>1.4008900116504479</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0907755352682578</v>
+        <v>1.1941121649252506</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28257,15 +28257,15 @@
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.5170982527352896E-4</v>
+        <v>8.9561239358659751E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5789899423973667E-4</v>
+        <v>1.4737239462375422E-4</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.715353844747188E-5</v>
+        <v>4.1064437231416293E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28294,11 +28294,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3075136612021857E-5</v>
+        <v>2.261363387978142E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3698674225107434E-5</v>
+        <v>1.3830392246502697E-5</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28318,55 +28318,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.156463254622671E-2</v>
+        <v>2.1776050512366189E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45028401885437597</v>
+        <v>0.43279726084061382</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0247593710066167</v>
+        <v>1.1218418377335595</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5115624164381969</v>
+        <v>1.4679596544255566</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5350071138153862</v>
+        <v>1.6629243733000019</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6674890961468525</v>
+        <v>1.6506457719433489</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4893672755441603</v>
+        <v>1.4746210648952083</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2055940126649165</v>
+        <v>1.1252210784872554</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.58992080522742829</v>
+        <v>0.62717896134705542</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.14581465407942715</v>
+        <v>0.14025981011449659</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.7805136626137011E-4</v>
+        <v>9.2195393457443866E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5037999451403492E-4</v>
+        <v>1.4887619456889457E-4</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.0282257474627412E-5</v>
+        <v>3.8717897961049643E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>

</xml_diff>